<commit_message>
added error checking and setup files
Added error checking to see if the IGS file is valid or not.

Created a setup.exe and setup.msi to install the program
</commit_message>
<xml_diff>
--- a/TaglistCreatorFromIGS/bin/Release/Resources/StandardTagList.xlsx
+++ b/TaglistCreatorFromIGS/bin/Release/Resources/StandardTagList.xlsx
@@ -5,14 +5,14 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212478881\Documents\Visual Studio 2015\Projects\TestConsoleApplication\TestConsoleApplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212478881\Documents\Visual Studio 2015\Projects\TaglistCreatorFromIGS\TaglistCreatorFromIGS\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="926"/>
   </bookViews>
   <sheets>
-    <sheet name="ZW1" sheetId="3" r:id="rId1"/>
+    <sheet name="Template" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -51,10 +51,10 @@
     <t>On-site Value</t>
   </si>
   <si>
-    <t>ZW1</t>
+    <t>Comments</t>
   </si>
   <si>
-    <t>Comments</t>
+    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -10097,11 +10097,12 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B6" sqref="B6:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -10156,7 +10157,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -10170,7 +10171,7 @@
     </row>
     <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -10236,9 +10237,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="E6" s="26"/>
       <c r="F6" s="32"/>
       <c r="G6" s="13"/>
@@ -10255,9 +10254,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
-      <c r="B7" s="4">
-        <v>3</v>
-      </c>
+      <c r="B7" s="4"/>
       <c r="E7" s="26"/>
       <c r="F7" s="32"/>
       <c r="G7" s="13"/>
@@ -10274,9 +10271,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="E8" s="27"/>
       <c r="F8" s="32"/>
       <c r="G8" s="13"/>
@@ -10293,9 +10288,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
-      <c r="B9" s="4">
-        <v>5</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="E9" s="26"/>
       <c r="F9" s="32"/>
       <c r="G9" s="5"/>
@@ -10312,9 +10305,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="4">
-        <v>6</v>
-      </c>
+      <c r="B10" s="4"/>
       <c r="E10" s="13"/>
       <c r="F10" s="32"/>
       <c r="G10" s="13"/>
@@ -10331,9 +10322,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="4">
-        <v>7</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="E11" s="13"/>
       <c r="F11" s="32"/>
       <c r="G11" s="13"/>
@@ -10350,9 +10339,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
-      <c r="B12" s="4">
-        <v>8</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="E12" s="13"/>
       <c r="F12" s="32"/>
       <c r="G12" s="13"/>
@@ -10369,9 +10356,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
-      <c r="B13" s="4">
-        <v>9</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="E13" s="6"/>
       <c r="F13" s="32"/>
       <c r="G13" s="13"/>
@@ -10388,9 +10373,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
-      <c r="B14" s="4">
-        <v>10</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="32"/>
       <c r="J14" s="4"/>
@@ -10405,9 +10388,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
-      <c r="B15" s="4">
-        <v>11</v>
-      </c>
+      <c r="B15" s="4"/>
       <c r="F15" s="32"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -10421,9 +10402,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
-      <c r="B16" s="4">
-        <v>12</v>
-      </c>
+      <c r="B16" s="4"/>
       <c r="F16" s="32"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -10437,9 +10416,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="4">
-        <v>13</v>
-      </c>
+      <c r="B17" s="4"/>
       <c r="E17" s="13"/>
       <c r="F17" s="30"/>
       <c r="G17" s="14"/>
@@ -10447,9 +10424,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
-      <c r="B18" s="4">
-        <v>14</v>
-      </c>
+      <c r="B18" s="4"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
@@ -10457,9 +10432,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
-      <c r="B19" s="4">
-        <v>15</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
@@ -10467,9 +10440,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
-      <c r="B20" s="4">
-        <v>16</v>
-      </c>
+      <c r="B20" s="4"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="14"/>
@@ -10477,9 +10448,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
-      <c r="B21" s="4">
-        <v>17</v>
-      </c>
+      <c r="B21" s="4"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -10487,9 +10456,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="4">
-        <v>18</v>
-      </c>
+      <c r="B22" s="4"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
@@ -10497,9 +10464,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
-      <c r="B23" s="4">
-        <v>19</v>
-      </c>
+      <c r="B23" s="4"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -10507,9 +10472,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="4">
-        <v>20</v>
-      </c>
+      <c r="B24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="13"/>
@@ -10517,9 +10480,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
-      <c r="B25" s="4">
-        <v>21</v>
-      </c>
+      <c r="B25" s="4"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="4"/>
@@ -10527,9 +10488,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
-      <c r="B26" s="4">
-        <v>22</v>
-      </c>
+      <c r="B26" s="4"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -10537,9 +10496,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="4">
-        <v>23</v>
-      </c>
+      <c r="B27" s="4"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -10547,9 +10504,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
-      <c r="B28" s="4">
-        <v>24</v>
-      </c>
+      <c r="B28" s="4"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="6"/>
@@ -10557,9 +10512,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
-      <c r="B29" s="4">
-        <v>25</v>
-      </c>
+      <c r="B29" s="4"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -10567,9 +10520,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="4">
-        <v>26</v>
-      </c>
+      <c r="B30" s="4"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
@@ -10577,9 +10528,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="4">
-        <v>27</v>
-      </c>
+      <c r="B31" s="4"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="15"/>
@@ -10587,181 +10536,135 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="4">
-        <v>28</v>
-      </c>
+      <c r="B32" s="4"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="15"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="4">
-        <v>29</v>
-      </c>
+      <c r="B33" s="4"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="15"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <v>30</v>
-      </c>
+      <c r="B34" s="4"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
-        <v>31</v>
-      </c>
+      <c r="B35" s="4"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="4">
-        <v>32</v>
-      </c>
+      <c r="B36" s="4"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="4">
-        <v>33</v>
-      </c>
+      <c r="B37" s="4"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="4">
-        <v>34</v>
-      </c>
+      <c r="B38" s="4"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="4">
-        <v>35</v>
-      </c>
+      <c r="B39" s="4"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="4">
-        <v>36</v>
-      </c>
+      <c r="B40" s="4"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="4">
-        <v>37</v>
-      </c>
+      <c r="B41" s="4"/>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="4">
-        <v>38</v>
-      </c>
+      <c r="B42" s="4"/>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="4">
-        <v>39</v>
-      </c>
+      <c r="B43" s="4"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="4">
-        <v>40</v>
-      </c>
+      <c r="B44" s="4"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="4">
-        <v>41</v>
-      </c>
+      <c r="B45" s="4"/>
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
-        <v>42</v>
-      </c>
+      <c r="B46" s="4"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="4">
-        <v>43</v>
-      </c>
+      <c r="B47" s="4"/>
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="4">
-        <v>44</v>
-      </c>
+      <c r="B48" s="4"/>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="4">
-        <v>45</v>
-      </c>
+      <c r="B49" s="4"/>
       <c r="E49" s="17"/>
       <c r="F49" s="17"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="4">
-        <v>46</v>
-      </c>
+      <c r="B50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="4">
-        <v>47</v>
-      </c>
+      <c r="B51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="4">
-        <v>48</v>
-      </c>
+      <c r="B52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="4">
-        <v>49</v>
-      </c>
+      <c r="B53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="4">
-        <v>50</v>
-      </c>
+      <c r="B54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>

</xml_diff>